<commit_message>
include feels as hnames
</commit_message>
<xml_diff>
--- a/docs/recodeBook.xlsx
+++ b/docs/recodeBook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="96">
   <si>
     <t xml:space="preserve">qname</t>
   </si>
@@ -162,6 +162,114 @@
   </si>
   <si>
     <t xml:space="preserve">Q122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.33_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anxious</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.32_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.33_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.32_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.33_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frustrated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.32_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.33_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Happy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.32_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.33_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.32_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.33_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ambivalent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.32_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.33_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surprised</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.32_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.33_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thankful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.32_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.33_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unhappy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.32_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.33_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worried</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.32_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.33_17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.32_17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.33_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3.32_10</t>
   </si>
   <si>
     <t xml:space="preserve">variable</t>
@@ -297,15 +405,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -490,6 +600,138 @@
       </c>
       <c r="B20" s="0" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -516,31 +758,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -548,7 +792,7 @@
         <v>45</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -556,7 +800,7 @@
         <v>42</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -564,15 +808,15 @@
         <v>26</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -580,7 +824,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -588,7 +832,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update names, move emotion vars
</commit_message>
<xml_diff>
--- a/docs/recodeBook.xlsx
+++ b/docs/recodeBook.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="94">
   <si>
     <t xml:space="preserve">qname</t>
   </si>
@@ -128,24 +129,24 @@
     <t xml:space="preserve">gender</t>
   </si>
   <si>
+    <t xml:space="preserve">Q3.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">becomeControl</t>
+  </si>
+  <si>
     <t xml:space="preserve">Q3.13</t>
   </si>
   <si>
-    <t xml:space="preserve">becomeControl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q3.12</t>
+    <t xml:space="preserve">Q2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avoidPreg</t>
   </si>
   <si>
     <t xml:space="preserve">Q2.7</t>
   </si>
   <si>
-    <t xml:space="preserve">avoidPreg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q2.2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Q3.5</t>
   </si>
   <si>
@@ -155,6 +156,48 @@
     <t xml:space="preserve">Q122</t>
   </si>
   <si>
+    <t xml:space="preserve">variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ageGroup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21-24; 25-29; 30-34; 35-39; 40-44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">underPovLevel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compare income category to poverty data and determine if under poverty level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">combine variables based on skip pattern (Q3.5 &amp; Q122) – can be planned in adv/in discussion w partner/to happen after ideal criteria = YES – just happens, left to fate or higher power, natural process meant to be = NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">combine variables based on skip pattern (Q2.2 &amp; Q2.5 for males, Q2.7 &amp; Q2.10 for females)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LowControl = no control, a little; HighControl = complete control, a lot of control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regionOrg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Region origin matched from state origin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Race where more than one response gets “other” category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of children</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REMOVED</t>
+  </si>
+  <si>
     <t xml:space="preserve">Q3.33_1</t>
   </si>
   <si>
@@ -261,45 +304,6 @@
   </si>
   <si>
     <t xml:space="preserve">Q3.32_10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">variable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ageGroup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-24; 25-29; 30-34; 35-39; 40-44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">underPovLevel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">compare income category to poverty data and determine if under poverty level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">combine variables based on skip pattern (Q3.5 &amp; Q122) – can be planned in adv/in discussion w partner/to happen after ideal criteria = YES – just happens, left to fate or higher power, natural process meant to be = NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">combine variables based on skip pattern (Q2.2 &amp; Q2.5 for males, Q2.7 &amp; Q2.10 for females)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LowControl = no control, a little; HighControl = complete control, a lot of control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regionOrg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Region origin matched from state origin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Race where more than one response gets “other” category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of children</t>
   </si>
 </sst>
 </file>
@@ -396,17 +400,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -580,138 +584,6 @@
       </c>
       <c r="B19" s="0" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -738,33 +610,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -772,7 +644,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -780,7 +652,7 @@
         <v>39</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -788,15 +660,15 @@
         <v>26</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -804,7 +676,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,7 +684,171 @@
         <v>12</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>92</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove commas from fields
</commit_message>
<xml_diff>
--- a/docs/recodeBook.xlsx
+++ b/docs/recodeBook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -174,13 +174,13 @@
     <t xml:space="preserve">compare income category to poverty data and determine if under poverty level</t>
   </si>
   <si>
-    <t xml:space="preserve">combine variables based on skip pattern (Q3.5 &amp; Q122) – can be planned in adv/in discussion w partner/to happen after ideal criteria = YES – just happens, left to fate or higher power, natural process meant to be = NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">combine variables based on skip pattern (Q2.2 &amp; Q2.5 for males, Q2.7 &amp; Q2.10 for females)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LowControl = no control, a little; HighControl = complete control, a lot of control</t>
+    <t xml:space="preserve">combine variables based on skip pattern (Q3.5 &amp; Q122) – can be planned in adv/in discussion w partner/to happen after ideal criteria = YES – just happens or left to fate or higher power or natural process meant to be = NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">combine variables based on skip pattern (Q2.2 &amp; Q2.5 for males or Q2.7 &amp; Q2.10 for females)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LowControl = no control or a little; HighControl = complete control or a lot of control</t>
   </si>
   <si>
     <t xml:space="preserve">regionOrg</t>
@@ -402,16 +402,16 @@
   </sheetPr>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -600,15 +600,15 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="174.678571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="172.790816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -715,7 +715,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>